<commit_message>
Changes solutions class 8
</commit_message>
<xml_diff>
--- a/Documents_files/FM250/Solution8_1.xlsx
+++ b/Documents_files/FM250/Solution8_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/domenicomergoni/Documents/LSE/Website_quarto/Documents_files/FM250/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37C77F78-F426-234E-9E23-3039EF6090CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AEC4338-4762-374C-A7D9-3771943A72C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3800" yWindow="620" windowWidth="21040" windowHeight="15840" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Revenues" sheetId="2" r:id="rId1"/>
@@ -229,7 +229,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -241,7 +241,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -560,7 +559,7 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -602,34 +601,34 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="17">
+      <c r="C2" s="16">
         <v>4.2</v>
       </c>
-      <c r="D2" s="17">
+      <c r="D2" s="16">
         <f>C2*1.05</f>
         <v>4.41</v>
       </c>
-      <c r="E2" s="17">
+      <c r="E2" s="16">
         <f t="shared" ref="E2:J2" si="0">D2*1.05</f>
         <v>4.6305000000000005</v>
       </c>
-      <c r="F2" s="17">
+      <c r="F2" s="16">
         <f t="shared" si="0"/>
         <v>4.8620250000000009</v>
       </c>
-      <c r="G2" s="17">
+      <c r="G2" s="16">
         <f t="shared" si="0"/>
         <v>5.1051262500000014</v>
       </c>
-      <c r="H2" s="17">
+      <c r="H2" s="16">
         <f t="shared" si="0"/>
         <v>5.3603825625000017</v>
       </c>
-      <c r="I2" s="17">
+      <c r="I2" s="16">
         <f t="shared" si="0"/>
         <v>5.6284016906250018</v>
       </c>
-      <c r="J2" s="17">
+      <c r="J2" s="16">
         <f t="shared" si="0"/>
         <v>5.9098217751562521</v>
       </c>
@@ -846,8 +845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5291ECF-C059-7F4F-B49B-414BDA2644A9}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView zoomScale="108" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1332,34 +1331,34 @@
         <v>8</v>
       </c>
       <c r="B20" s="4"/>
-      <c r="C20" s="9">
+      <c r="C20" s="4">
         <v>0.1</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20" s="4">
         <f>C20*1.04</f>
         <v>0.10400000000000001</v>
       </c>
-      <c r="E20" s="9">
+      <c r="E20" s="4">
         <f t="shared" ref="E20:J20" si="7">D20*1.04</f>
         <v>0.10816000000000002</v>
       </c>
-      <c r="F20" s="9">
+      <c r="F20" s="4">
         <f t="shared" si="7"/>
         <v>0.11248640000000003</v>
       </c>
-      <c r="G20" s="9">
+      <c r="G20" s="4">
         <f t="shared" si="7"/>
         <v>0.11698585600000003</v>
       </c>
-      <c r="H20" s="9">
+      <c r="H20" s="4">
         <f t="shared" si="7"/>
         <v>0.12166529024000003</v>
       </c>
-      <c r="I20" s="9">
+      <c r="I20" s="4">
         <f t="shared" si="7"/>
         <v>0.12653190184960003</v>
       </c>
-      <c r="J20" s="9">
+      <c r="J20" s="4">
         <f t="shared" si="7"/>
         <v>0.13159317792358405</v>
       </c>
@@ -1369,35 +1368,35 @@
         <v>9</v>
       </c>
       <c r="B21" s="4"/>
-      <c r="C21" s="9">
+      <c r="C21" s="4">
         <f>C20*0.35</f>
         <v>3.4999999999999996E-2</v>
       </c>
-      <c r="D21" s="9">
+      <c r="D21" s="4">
         <f t="shared" ref="D21:J21" si="8">D20*0.35</f>
         <v>3.6400000000000002E-2</v>
       </c>
-      <c r="E21" s="9">
+      <c r="E21" s="4">
         <f t="shared" si="8"/>
         <v>3.7856000000000008E-2</v>
       </c>
-      <c r="F21" s="9">
+      <c r="F21" s="4">
         <f t="shared" si="8"/>
         <v>3.9370240000000008E-2</v>
       </c>
-      <c r="G21" s="9">
+      <c r="G21" s="4">
         <f t="shared" si="8"/>
         <v>4.0945049600000005E-2</v>
       </c>
-      <c r="H21" s="9">
+      <c r="H21" s="4">
         <f t="shared" si="8"/>
         <v>4.2582851584000006E-2</v>
       </c>
-      <c r="I21" s="9">
+      <c r="I21" s="4">
         <f t="shared" si="8"/>
         <v>4.4286165647360008E-2</v>
       </c>
-      <c r="J21" s="9">
+      <c r="J21" s="4">
         <f t="shared" si="8"/>
         <v>4.6057612273254417E-2</v>
       </c>
@@ -1407,87 +1406,87 @@
         <v>10</v>
       </c>
       <c r="B22" s="4"/>
-      <c r="C22" s="9">
+      <c r="C22" s="4">
         <f>C20-C21</f>
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="D22" s="9">
+      <c r="D22" s="4">
         <f t="shared" ref="D22:J22" si="9">D20-D21</f>
         <v>6.7600000000000007E-2</v>
       </c>
-      <c r="E22" s="9">
+      <c r="E22" s="4">
         <f t="shared" si="9"/>
         <v>7.0304000000000005E-2</v>
       </c>
-      <c r="F22" s="9">
+      <c r="F22" s="4">
         <f t="shared" si="9"/>
         <v>7.3116160000000013E-2</v>
       </c>
-      <c r="G22" s="9">
+      <c r="G22" s="4">
         <f t="shared" si="9"/>
         <v>7.6040806400000022E-2</v>
       </c>
-      <c r="H22" s="9">
+      <c r="H22" s="4">
         <f t="shared" si="9"/>
         <v>7.9082438656000023E-2</v>
       </c>
-      <c r="I22" s="9">
+      <c r="I22" s="4">
         <f t="shared" si="9"/>
         <v>8.2245736202240016E-2</v>
       </c>
-      <c r="J22" s="9">
+      <c r="J22" s="4">
         <f t="shared" si="9"/>
         <v>8.5535565650329631E-2</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B23" s="4"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>20</v>
       </c>
-      <c r="B24" s="16">
+      <c r="B24" s="15">
         <f>B7-B9-B18-B22</f>
         <v>-1.5499999999999998</v>
       </c>
-      <c r="C24" s="16">
+      <c r="C24" s="15">
         <f>C7-C9-C18-C22</f>
         <v>0.17999999999999988</v>
       </c>
-      <c r="D24" s="16">
+      <c r="D24" s="15">
         <f t="shared" ref="D24:I24" si="10">D7-D9-D18-D22</f>
         <v>0.24004999999999987</v>
       </c>
-      <c r="E24" s="16">
+      <c r="E24" s="15">
         <f t="shared" si="10"/>
         <v>0.25062849999999992</v>
       </c>
-      <c r="F24" s="16">
+      <c r="F24" s="15">
         <f t="shared" si="10"/>
         <v>0.26176296500000007</v>
       </c>
-      <c r="G24" s="16">
+      <c r="G24" s="15">
         <f t="shared" si="10"/>
         <v>0.27348227484999965</v>
       </c>
-      <c r="H24" s="16">
+      <c r="H24" s="15">
         <f t="shared" si="10"/>
         <v>0.28581679665650017</v>
       </c>
-      <c r="I24" s="16">
+      <c r="I24" s="15">
         <f t="shared" si="10"/>
         <v>0.2987984608758853</v>
       </c>
-      <c r="J24" s="16">
+      <c r="J24" s="15">
         <f>J7-J9-J18-J22+J15</f>
         <v>1.2474430187973269</v>
       </c>
@@ -1496,39 +1495,39 @@
       <c r="A25" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="16">
+      <c r="B25" s="15">
         <f>B24/1.12^B1</f>
         <v>-1.5499999999999998</v>
       </c>
-      <c r="C25" s="16">
+      <c r="C25" s="15">
         <f t="shared" ref="C25:J25" si="11">C24/1.12^C1</f>
         <v>0.16071428571428559</v>
       </c>
-      <c r="D25" s="16">
+      <c r="D25" s="15">
         <f t="shared" si="11"/>
         <v>0.19136639030612232</v>
       </c>
-      <c r="E25" s="16">
+      <c r="E25" s="15">
         <f t="shared" si="11"/>
         <v>0.1783924158391034</v>
       </c>
-      <c r="F25" s="16">
+      <c r="F25" s="15">
         <f t="shared" si="11"/>
         <v>0.16635509651435113</v>
       </c>
-      <c r="G25" s="16">
+      <c r="G25" s="15">
         <f t="shared" si="11"/>
         <v>0.15518118731290506</v>
       </c>
-      <c r="H25" s="16">
+      <c r="H25" s="15">
         <f t="shared" si="11"/>
         <v>0.14480368414139297</v>
       </c>
-      <c r="I25" s="16">
+      <c r="I25" s="15">
         <f t="shared" si="11"/>
         <v>0.13516124932107818</v>
       </c>
-      <c r="J25" s="16">
+      <c r="J25" s="15">
         <f t="shared" si="11"/>
         <v>0.50382131315219325</v>
       </c>
@@ -1537,7 +1536,7 @@
       <c r="A26" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="16">
+      <c r="B26" s="15">
         <f>SUM(B25:J25)</f>
         <v>8.5795622301432117E-2</v>
       </c>
@@ -2427,7 +2426,7 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2505,35 +2504,35 @@
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="18">
+      <c r="C3" s="17">
         <f>C2*0.9</f>
         <v>3.7800000000000002</v>
       </c>
-      <c r="D3" s="18">
+      <c r="D3" s="17">
         <f t="shared" ref="D3:J3" si="1">D2*0.9</f>
         <v>3.9690000000000003</v>
       </c>
-      <c r="E3" s="18">
+      <c r="E3" s="17">
         <f t="shared" si="1"/>
         <v>4.1674500000000005</v>
       </c>
-      <c r="F3" s="18">
+      <c r="F3" s="17">
         <f t="shared" si="1"/>
         <v>4.3758225000000008</v>
       </c>
-      <c r="G3" s="18">
+      <c r="G3" s="17">
         <f t="shared" si="1"/>
         <v>4.5946136250000018</v>
       </c>
-      <c r="H3" s="18">
+      <c r="H3" s="17">
         <f t="shared" si="1"/>
         <v>4.8243443062500013</v>
       </c>
-      <c r="I3" s="18">
+      <c r="I3" s="17">
         <f t="shared" si="1"/>
         <v>5.0655615215625014</v>
       </c>
-      <c r="J3" s="18">
+      <c r="J3" s="17">
         <f t="shared" si="1"/>
         <v>5.3188395976406273</v>
       </c>
@@ -2741,7 +2740,7 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView zoomScale="157" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2856,28 +2855,28 @@
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="10">
-        <v>0.12</v>
-      </c>
-      <c r="D4" s="10">
-        <v>0.12</v>
-      </c>
-      <c r="E4" s="10">
-        <v>0.12</v>
-      </c>
-      <c r="F4" s="10">
-        <v>0.12</v>
-      </c>
-      <c r="G4" s="10">
-        <v>0.12</v>
-      </c>
-      <c r="H4" s="10">
-        <v>0.12</v>
-      </c>
-      <c r="I4" s="10">
-        <v>0.12</v>
-      </c>
-      <c r="J4" s="10">
+      <c r="C4" s="9">
+        <v>0.12</v>
+      </c>
+      <c r="D4" s="9">
+        <v>0.12</v>
+      </c>
+      <c r="E4" s="9">
+        <v>0.12</v>
+      </c>
+      <c r="F4" s="9">
+        <v>0.12</v>
+      </c>
+      <c r="G4" s="9">
+        <v>0.12</v>
+      </c>
+      <c r="H4" s="9">
+        <v>0.12</v>
+      </c>
+      <c r="I4" s="9">
+        <v>0.12</v>
+      </c>
+      <c r="J4" s="9">
         <v>0.12</v>
       </c>
     </row>
@@ -3436,7 +3435,7 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView zoomScale="225" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3616,35 +3615,35 @@
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="10">
         <f>C5*(1-0.35)</f>
         <v>0.19499999999999995</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="10">
         <f t="shared" ref="D6:J6" si="3">D5*(1-0.35)</f>
         <v>0.20864999999999989</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="10">
         <f t="shared" si="3"/>
         <v>0.22298249999999997</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="10">
         <f t="shared" si="3"/>
         <v>0.23803162500000008</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="10">
         <f t="shared" si="3"/>
         <v>0.25383320624999978</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="10">
         <f t="shared" si="3"/>
         <v>0.27042486656250025</v>
       </c>
-      <c r="I6" s="11">
+      <c r="I6" s="10">
         <f t="shared" si="3"/>
         <v>0.28784610989062531</v>
       </c>
-      <c r="J6" s="11">
+      <c r="J6" s="10">
         <f t="shared" si="3"/>
         <v>0.30613841538515613</v>
       </c>
@@ -4043,35 +4042,35 @@
       <c r="A7" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="12">
         <f>C6+C4</f>
         <v>0.31499999999999995</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7" s="12">
         <f t="shared" ref="D7:J7" si="4">D6+D4</f>
         <v>0.32864999999999989</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="12">
         <f t="shared" si="4"/>
         <v>0.34298249999999997</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="12">
         <f t="shared" si="4"/>
         <v>0.35803162500000008</v>
       </c>
-      <c r="G7" s="13">
+      <c r="G7" s="12">
         <f t="shared" si="4"/>
         <v>0.37383320624999977</v>
       </c>
-      <c r="H7" s="13">
+      <c r="H7" s="12">
         <f t="shared" si="4"/>
         <v>0.39042486656250025</v>
       </c>
-      <c r="I7" s="13">
+      <c r="I7" s="12">
         <f t="shared" si="4"/>
         <v>0.40784610989062531</v>
       </c>
-      <c r="J7" s="13">
+      <c r="J7" s="12">
         <f t="shared" si="4"/>
         <v>0.42613841538515612</v>
       </c>
@@ -4242,7 +4241,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView zoomScale="200" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4507,7 +4506,7 @@
       <c r="A9" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="14">
+      <c r="B9" s="13">
         <v>1.2</v>
       </c>
     </row>
@@ -4534,7 +4533,7 @@
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
-      <c r="J11" s="12">
+      <c r="J11" s="11">
         <f>B9-SUM(C4:J4)</f>
         <v>0.24</v>
       </c>
@@ -4551,7 +4550,7 @@
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
-      <c r="J12" s="12">
+      <c r="J12" s="11">
         <v>0.4</v>
       </c>
     </row>
@@ -4567,7 +4566,7 @@
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
-      <c r="J13" s="12">
+      <c r="J13" s="11">
         <f>J12-J11</f>
         <v>0.16000000000000003</v>
       </c>
@@ -4584,7 +4583,7 @@
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
-      <c r="J14" s="12">
+      <c r="J14" s="11">
         <f>J13*0.35</f>
         <v>5.6000000000000008E-2</v>
       </c>
@@ -4601,7 +4600,7 @@
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
-      <c r="J15" s="12">
+      <c r="J15" s="11">
         <f>J12-J14</f>
         <v>0.34400000000000003</v>
       </c>
@@ -5066,38 +5065,38 @@
       <c r="A17" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="19">
+      <c r="B17" s="18">
         <v>0.35</v>
       </c>
-      <c r="C17" s="20">
+      <c r="C17" s="19">
         <f t="shared" ref="C17:I17" si="5">0.1*C2</f>
         <v>0.42000000000000004</v>
       </c>
-      <c r="D17" s="20">
+      <c r="D17" s="19">
         <f t="shared" si="5"/>
         <v>0.44100000000000006</v>
       </c>
-      <c r="E17" s="20">
+      <c r="E17" s="19">
         <f t="shared" si="5"/>
         <v>0.46305000000000007</v>
       </c>
-      <c r="F17" s="20">
+      <c r="F17" s="19">
         <f t="shared" si="5"/>
         <v>0.48620250000000009</v>
       </c>
-      <c r="G17" s="20">
+      <c r="G17" s="19">
         <f t="shared" si="5"/>
         <v>0.51051262500000016</v>
       </c>
-      <c r="H17" s="20">
+      <c r="H17" s="19">
         <f t="shared" si="5"/>
         <v>0.53603825625000023</v>
       </c>
-      <c r="I17" s="20">
+      <c r="I17" s="19">
         <f t="shared" si="5"/>
         <v>0.56284016906250023</v>
       </c>
-      <c r="J17" s="20">
+      <c r="J17" s="19">
         <v>0</v>
       </c>
     </row>
@@ -5105,39 +5104,39 @@
       <c r="A18" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="19">
+      <c r="B18" s="18">
         <f>B17</f>
         <v>0.35</v>
       </c>
-      <c r="C18" s="20">
+      <c r="C18" s="19">
         <f>C17-B17</f>
         <v>7.0000000000000062E-2</v>
       </c>
-      <c r="D18" s="20">
+      <c r="D18" s="19">
         <f t="shared" ref="D18:J18" si="6">D17-C17</f>
         <v>2.1000000000000019E-2</v>
       </c>
-      <c r="E18" s="20">
+      <c r="E18" s="19">
         <f t="shared" si="6"/>
         <v>2.2050000000000014E-2</v>
       </c>
-      <c r="F18" s="20">
+      <c r="F18" s="19">
         <f t="shared" si="6"/>
         <v>2.315250000000002E-2</v>
       </c>
-      <c r="G18" s="20">
+      <c r="G18" s="19">
         <f t="shared" si="6"/>
         <v>2.4310125000000071E-2</v>
       </c>
-      <c r="H18" s="20">
+      <c r="H18" s="19">
         <f t="shared" si="6"/>
         <v>2.5525631250000069E-2</v>
       </c>
-      <c r="I18" s="20">
+      <c r="I18" s="19">
         <f t="shared" si="6"/>
         <v>2.6801912812499995E-2</v>
       </c>
-      <c r="J18" s="20">
+      <c r="J18" s="19">
         <f t="shared" si="6"/>
         <v>-0.56284016906250023</v>
       </c>
@@ -5593,34 +5592,34 @@
       <c r="A19" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="15">
+      <c r="C19" s="14">
         <v>0.1</v>
       </c>
-      <c r="D19" s="15">
+      <c r="D19" s="14">
         <f>C19*1.04</f>
         <v>0.10400000000000001</v>
       </c>
-      <c r="E19" s="15">
+      <c r="E19" s="14">
         <f t="shared" ref="E19:J19" si="7">D19*1.04</f>
         <v>0.10816000000000002</v>
       </c>
-      <c r="F19" s="15">
+      <c r="F19" s="14">
         <f t="shared" si="7"/>
         <v>0.11248640000000003</v>
       </c>
-      <c r="G19" s="15">
+      <c r="G19" s="14">
         <f t="shared" si="7"/>
         <v>0.11698585600000003</v>
       </c>
-      <c r="H19" s="15">
+      <c r="H19" s="14">
         <f t="shared" si="7"/>
         <v>0.12166529024000003</v>
       </c>
-      <c r="I19" s="15">
+      <c r="I19" s="14">
         <f t="shared" si="7"/>
         <v>0.12653190184960003</v>
       </c>
-      <c r="J19" s="15">
+      <c r="J19" s="14">
         <f t="shared" si="7"/>
         <v>0.13159317792358405</v>
       </c>
@@ -5629,35 +5628,35 @@
       <c r="A20" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="15">
+      <c r="C20" s="14">
         <f>C19*0.35</f>
         <v>3.4999999999999996E-2</v>
       </c>
-      <c r="D20" s="15">
+      <c r="D20" s="14">
         <f t="shared" ref="D20:J20" si="8">D19*0.35</f>
         <v>3.6400000000000002E-2</v>
       </c>
-      <c r="E20" s="15">
+      <c r="E20" s="14">
         <f t="shared" si="8"/>
         <v>3.7856000000000008E-2</v>
       </c>
-      <c r="F20" s="15">
+      <c r="F20" s="14">
         <f t="shared" si="8"/>
         <v>3.9370240000000008E-2</v>
       </c>
-      <c r="G20" s="15">
+      <c r="G20" s="14">
         <f t="shared" si="8"/>
         <v>4.0945049600000005E-2</v>
       </c>
-      <c r="H20" s="15">
+      <c r="H20" s="14">
         <f t="shared" si="8"/>
         <v>4.2582851584000006E-2</v>
       </c>
-      <c r="I20" s="15">
+      <c r="I20" s="14">
         <f t="shared" si="8"/>
         <v>4.4286165647360008E-2</v>
       </c>
-      <c r="J20" s="15">
+      <c r="J20" s="14">
         <f t="shared" si="8"/>
         <v>4.6057612273254417E-2</v>
       </c>
@@ -5666,35 +5665,35 @@
       <c r="A21" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="15">
+      <c r="C21" s="14">
         <f>C19-C20</f>
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="D21" s="15">
+      <c r="D21" s="14">
         <f t="shared" ref="D21:J21" si="9">D19-D20</f>
         <v>6.7600000000000007E-2</v>
       </c>
-      <c r="E21" s="15">
+      <c r="E21" s="14">
         <f t="shared" si="9"/>
         <v>7.0304000000000005E-2</v>
       </c>
-      <c r="F21" s="15">
+      <c r="F21" s="14">
         <f t="shared" si="9"/>
         <v>7.3116160000000013E-2</v>
       </c>
-      <c r="G21" s="15">
+      <c r="G21" s="14">
         <f t="shared" si="9"/>
         <v>7.6040806400000022E-2</v>
       </c>
-      <c r="H21" s="15">
+      <c r="H21" s="14">
         <f t="shared" si="9"/>
         <v>7.9082438656000023E-2</v>
       </c>
-      <c r="I21" s="15">
+      <c r="I21" s="14">
         <f t="shared" si="9"/>
         <v>8.2245736202240016E-2</v>
       </c>
-      <c r="J21" s="15">
+      <c r="J21" s="14">
         <f t="shared" si="9"/>
         <v>8.5535565650329631E-2</v>
       </c>

</xml_diff>